<commit_message>
revised abstract, methods, personnel
</commit_message>
<xml_diff>
--- a/nes-lter-zooplankton-transect-abundance-335um-info.xlsx
+++ b/nes-lter-zooplankton-transect-abundance-335um-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-zooplankton-transect-abundance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0F1DEC-8EFA-4428-820B-2E43D5D25075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{560E92C8-BB78-4D6E-8DFF-40178ED9ECC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29205" yWindow="2640" windowWidth="23250" windowHeight="14010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="2" r:id="rId1"/>
@@ -19,13 +19,13 @@
   </sheets>
   <calcPr calcId="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Filter 1" guid="{DCA8ADC8-581D-4138-A617-9AD802A378C1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{B6505D7F-CDEF-4B2C-9A38-AC64B4FD4F4B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="96">
   <si>
     <t>cruise</t>
   </si>
@@ -213,27 +213,27 @@
     <t>OCE-1655686</t>
   </si>
   <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Richardson</t>
+  </si>
+  <si>
+    <t>Northeast Fisheries Science Center</t>
+  </si>
+  <si>
+    <t>NOAA</t>
+  </si>
+  <si>
+    <t>EcoMon</t>
+  </si>
+  <si>
     <t>PI</t>
   </si>
   <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>Richardson</t>
-  </si>
-  <si>
-    <t>Northeast Fisheries Science Center</t>
-  </si>
-  <si>
-    <t>NOAA</t>
-  </si>
-  <si>
-    <t>EcoMon</t>
-  </si>
-  <si>
     <t>NES-LTER Information Manager</t>
   </si>
   <si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>technician</t>
+  </si>
+  <si>
+    <t>Harvey</t>
+  </si>
+  <si>
+    <t>Walsh</t>
   </si>
   <si>
     <t>keyword</t>
@@ -651,7 +657,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +678,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -693,7 +699,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -714,7 +720,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="13.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -734,7 +740,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -754,7 +760,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="13.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -774,7 +780,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -794,7 +800,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="13.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -814,7 +820,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="13.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -834,7 +840,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="13.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -854,7 +860,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="13.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -874,7 +880,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="13.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -894,7 +900,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="13.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -914,7 +920,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="13.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -934,7 +940,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="13.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -954,7 +960,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="13.2">
+    <row r="18" spans="2:2">
       <c r="B18" s="5"/>
     </row>
   </sheetData>
@@ -967,11 +973,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -1044,16 +1048,16 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1064,10 +1068,10 @@
         <v>56</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1090,7 +1094,7 @@
         <v>58</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>56</v>
@@ -1104,30 +1108,30 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>56</v>
       </c>
       <c r="I5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1186,6 +1190,29 @@
       </c>
       <c r="J7" s="4" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1209,82 +1236,82 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="9:9">

</xml_diff>